<commit_message>
Flow graph output to GML, optimizations, bugs & changes
Flow graph output to GML.
Optimizations after a profiling
Reorganization and basic implementation of output results RESTful calls 
Reset state on each file submission (RESTful call)
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/Biofuel_NIS.xlsx
+++ b/backend_tests/z_input_files/v2/Biofuel_NIS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="InterfaceTypes" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="172">
   <si>
     <t xml:space="preserve">InterfaceTypeHierarchy</t>
   </si>
@@ -487,6 +487,9 @@
     <t xml:space="preserve">Scale</t>
   </si>
   <si>
+    <t xml:space="preserve">? p1&lt;0.3 =&gt; 0.5, p1&gt;=0.3 AND p1&lt;0.7 =&gt; 0, true =&gt; 0.3 ?</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.4*10</t>
   </si>
   <si>
@@ -530,6 +533,9 @@
   </si>
   <si>
     <t xml:space="preserve">avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DummyCol</t>
   </si>
   <si>
     <t xml:space="preserve">PalmOil1</t>
@@ -691,6 +697,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="10" style="0" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1297,10 +1304,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1308,6 +1315,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>17</v>
@@ -1316,7 +1328,7 @@
         <v>101</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>17</v>
@@ -1325,7 +1337,7 @@
         <v>130</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
@@ -1339,7 +1351,7 @@
         <v>101</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>17</v>
@@ -1348,13 +1360,13 @@
         <v>130</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>68</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -5143,10 +5155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5202,6 +5214,9 @@
       <c r="G2" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -5240,7 +5255,7 @@
         <v>101</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5471,7 +5486,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>27</v>
@@ -5480,7 +5495,7 @@
         <v>27</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>0.1</v>
@@ -5494,7 +5509,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>29</v>
@@ -5503,7 +5518,7 @@
         <v>29</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>0.2</v>
@@ -5517,7 +5532,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>27</v>
@@ -5540,7 +5555,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>29</v>
@@ -5563,7 +5578,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>23</v>
@@ -5572,7 +5587,7 @@
         <v>23</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0.7</v>
@@ -5586,7 +5601,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>25</v>
@@ -5595,7 +5610,7 @@
         <v>25</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>0.8</v>
@@ -5609,7 +5624,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>23</v>
@@ -5632,7 +5647,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>25</v>
@@ -5655,7 +5670,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>17</v>
@@ -5664,7 +5679,7 @@
         <v>17</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>0.8</v>
@@ -5678,7 +5693,7 @@
         <v>101</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>130</v>
@@ -5687,7 +5702,7 @@
         <v>130</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>0.9</v>
@@ -5701,7 +5716,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>21</v>
@@ -5710,7 +5725,7 @@
         <v>21</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>0.7</v>
@@ -5724,7 +5739,7 @@
         <v>17</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>17</v>
@@ -5747,7 +5762,7 @@
         <v>101</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>130</v>
@@ -5770,7 +5785,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>21</v>
@@ -5793,7 +5808,7 @@
         <v>94</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>31</v>
@@ -5802,7 +5817,7 @@
         <v>27</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>0.2</v>
@@ -5813,7 +5828,7 @@
         <v>31</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>151</v>
@@ -5836,7 +5851,7 @@
         <v>96</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>31</v>
@@ -5845,7 +5860,7 @@
         <v>23</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>0.8</v>
@@ -5856,7 +5871,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>151</v>
@@ -5879,7 +5894,7 @@
         <v>97</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>32</v>
@@ -5962,7 +5977,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>60</v>
@@ -5976,7 +5991,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>65</v>
@@ -5987,7 +6002,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>65</v>
@@ -5998,7 +6013,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Refactoring flow graph solver. Refactored Issue class.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/Biofuel_NIS.xlsx
+++ b/backend_tests/z_input_files/v2/Biofuel_NIS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="183">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -144,7 +144,7 @@
     <t xml:space="preserve">PalmFruit</t>
   </si>
   <si>
-    <t xml:space="preserve">Rapeseed</t>
+    <t xml:space="preserve">RapeSeed</t>
   </si>
   <si>
     <t xml:space="preserve">SoyBean</t>
@@ -357,9 +357,6 @@
     <t xml:space="preserve">Archetype</t>
   </si>
   <si>
-    <t xml:space="preserve">RapeSeed</t>
-  </si>
-  <si>
     <t xml:space="preserve">“n-3”</t>
   </si>
   <si>
@@ -451,9 +448,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sugarbeet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RapeseedCrop</t>
   </si>
   <si>
     <t xml:space="preserve">OriginProcessors</t>
@@ -690,7 +684,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -739,14 +733,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -761,10 +747,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1276,7 +1258,7 @@
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1780,7 +1762,7 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2086,7 +2068,7 @@
         <v>105</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>107</v>
@@ -2179,10 +2161,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>106</v>
@@ -2196,10 +2178,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>106</v>
@@ -2213,13 +2195,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>107</v>
@@ -2230,13 +2212,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>107</v>
@@ -2247,10 +2229,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>39</v>
@@ -2264,10 +2246,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>39</v>
@@ -2281,10 +2263,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>40</v>
@@ -2298,10 +2280,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>40</v>
@@ -2315,10 +2297,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>41</v>
@@ -2332,10 +2314,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>41</v>
@@ -2349,10 +2331,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>42</v>
@@ -2366,10 +2348,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>42</v>
@@ -2383,10 +2365,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>43</v>
@@ -2400,10 +2382,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>43</v>
@@ -2472,7 +2454,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>79</v>
@@ -2484,7 +2466,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>31</v>
@@ -2496,7 +2478,7 @@
         <v>90</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>3</v>
@@ -2505,31 +2487,31 @@
         <v>30</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2540,7 +2522,7 @@
         <v>92</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L2" s="0"/>
       <c r="S2" s="0"/>
@@ -2557,7 +2539,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L3" s="0"/>
       <c r="S3" s="0"/>
@@ -2570,13 +2552,13 @@
         <v>47</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2591,13 +2573,13 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>9</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,13 +2590,13 @@
         <v>98</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>10</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2625,13 +2607,13 @@
         <v>98</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>11</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2642,7 +2624,7 @@
         <v>100</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L8" s="0"/>
     </row>
@@ -2658,125 +2640,125 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="L9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="L9" s="0"/>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="12" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13" t="s">
+      <c r="G11" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="G13" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="D14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="G15" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="G16" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="G17" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13" t="s">
+      <c r="G18" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13" t="s">
-        <v>138</v>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,21 +2766,21 @@
         <v>37</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2806,10 +2788,10 @@
         <v>39</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2817,10 +2799,10 @@
         <v>40</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,10 +2810,10 @@
         <v>41</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2839,10 +2821,10 @@
         <v>42</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,12 +2833,12 @@
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2864,153 +2846,153 @@
         <v>37</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G27" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="12" t="s">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G29" s="12" t="s">
+      <c r="D30" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="30" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="12" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="G31" s="12" t="s">
+      <c r="D32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="32" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="12" t="s">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="12" t="s">
+      <c r="D33" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="34" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="12" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G35" s="12" t="s">
+      <c r="D35" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="36" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="12" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G37" s="12" t="s">
+      <c r="D37" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="39" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="12" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="G39" s="12" t="s">
+      <c r="D39" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" s="4" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="40" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3031,8 +3013,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L50" activeCellId="0" sqref="L50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3068,7 +3050,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>79</v>
@@ -3080,7 +3062,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>31</v>
@@ -3092,7 +3074,7 @@
         <v>90</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>3</v>
@@ -3101,31 +3083,31 @@
         <v>30</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,10 +3115,10 @@
         <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L2" s="4" t="n">
         <v>0.1285149</v>
@@ -3153,10 +3135,10 @@
         <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L3" s="4" t="n">
         <v>0.1164551</v>
@@ -3173,10 +3155,10 @@
         <v>48</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L4" s="4" t="n">
         <v>0.1144008</v>
@@ -3193,10 +3175,10 @@
         <v>48</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L5" s="4" t="n">
         <v>0.0810668396092578</v>
@@ -3213,10 +3195,10 @@
         <v>48</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L6" s="4" t="n">
         <v>0.0810241451952682</v>
@@ -3233,10 +3215,10 @@
         <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L7" s="4" t="n">
         <v>0.0837198399276661</v>
@@ -3253,16 +3235,16 @@
         <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L8" s="4" t="n">
         <v>0.0125177909103313</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S8" s="4" t="n">
         <v>2011</v>
@@ -3273,16 +3255,16 @@
         <v>48</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L9" s="4" t="n">
         <v>0.0125698253799858</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S9" s="4" t="n">
         <v>2012</v>
@@ -3293,16 +3275,16 @@
         <v>48</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L10" s="4" t="n">
         <v>0.012779585379132</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S10" s="4" t="n">
         <v>2013</v>
@@ -3313,10 +3295,10 @@
         <v>48</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L11" s="4" t="n">
         <v>0.290807572629191</v>
@@ -3333,10 +3315,10 @@
         <v>48</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L12" s="4" t="n">
         <v>0.284819139846198</v>
@@ -3353,10 +3335,10 @@
         <v>48</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L13" s="4" t="n">
         <v>0.338398023755541</v>
@@ -3373,10 +3355,10 @@
         <v>54</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L14" s="4" t="n">
         <v>510.783090193891</v>
@@ -3393,10 +3375,10 @@
         <v>54</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L15" s="4" t="n">
         <v>510.783090193891</v>
@@ -3413,10 +3395,10 @@
         <v>54</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L16" s="4" t="n">
         <v>510.783090193891</v>
@@ -3433,10 +3415,10 @@
         <v>54</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L17" s="4" t="n">
         <v>344.554124680908</v>
@@ -3453,10 +3435,10 @@
         <v>54</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L18" s="4" t="n">
         <v>344.554124680908</v>
@@ -3473,10 +3455,10 @@
         <v>54</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L19" s="4" t="n">
         <v>344.554124680908</v>
@@ -3493,16 +3475,16 @@
         <v>54</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L20" s="4" t="n">
         <v>54.7726040228444</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S20" s="4" t="n">
         <v>2011</v>
@@ -3513,16 +3495,16 @@
         <v>54</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L21" s="4" t="n">
         <v>54.7726040228444</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S21" s="4" t="n">
         <v>2012</v>
@@ -3533,16 +3515,16 @@
         <v>54</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L22" s="4" t="n">
         <v>54.7726040228444</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S22" s="4" t="n">
         <v>2013</v>
@@ -3553,10 +3535,10 @@
         <v>54</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L23" s="4" t="n">
         <v>876.195771627155</v>
@@ -3573,10 +3555,10 @@
         <v>54</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L24" s="4" t="n">
         <v>876.195771627155</v>
@@ -3593,10 +3575,10 @@
         <v>54</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L25" s="4" t="n">
         <v>876.195771627155</v>
@@ -3613,10 +3595,10 @@
         <v>57</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>42</v>
@@ -3630,10 +3612,10 @@
         <v>57</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>42</v>
@@ -3647,10 +3629,10 @@
         <v>57</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>42</v>
@@ -3664,10 +3646,10 @@
         <v>57</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L29" s="4" t="n">
         <v>16.2712344327208</v>
@@ -3684,10 +3666,10 @@
         <v>57</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L30" s="4" t="n">
         <v>16.2712344327208</v>
@@ -3704,10 +3686,10 @@
         <v>57</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L31" s="4" t="n">
         <v>16.2712344327208</v>
@@ -3724,16 +3706,16 @@
         <v>57</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L32" s="4" t="n">
         <v>0.219509168287431</v>
       </c>
       <c r="R32" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S32" s="4" t="n">
         <v>2011</v>
@@ -3744,16 +3726,16 @@
         <v>57</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L33" s="4" t="n">
         <v>0.219509168287431</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S33" s="4" t="n">
         <v>2012</v>
@@ -3764,16 +3746,16 @@
         <v>57</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L34" s="4" t="n">
         <v>0.219509168287431</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S34" s="4" t="n">
         <v>2013</v>
@@ -3784,10 +3766,10 @@
         <v>57</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>38</v>
@@ -3801,10 +3783,10 @@
         <v>57</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>38</v>
@@ -3818,10 +3800,10 @@
         <v>57</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>38</v>
@@ -3835,10 +3817,10 @@
         <v>59</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L38" s="4" t="n">
         <v>1.7056684219636</v>
@@ -3855,10 +3837,10 @@
         <v>59</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L39" s="4" t="n">
         <v>1.53914935457665</v>
@@ -3875,10 +3857,10 @@
         <v>59</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L40" s="4" t="n">
         <v>1.49408548045622</v>
@@ -3895,10 +3877,10 @@
         <v>59</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L41" s="4" t="n">
         <v>1.07593102225148</v>
@@ -3915,10 +3897,10 @@
         <v>59</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L42" s="4" t="n">
         <v>1.07086983533865</v>
@@ -3935,10 +3917,10 @@
         <v>59</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L43" s="4" t="n">
         <v>1.09338948158698</v>
@@ -3955,16 +3937,16 @@
         <v>59</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L44" s="4" t="n">
         <v>0.304586264843106</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S44" s="4" t="n">
         <v>2011</v>
@@ -3975,16 +3957,16 @@
         <v>59</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L45" s="4" t="n">
         <v>0.304574055933306</v>
       </c>
       <c r="R45" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S45" s="4" t="n">
         <v>2012</v>
@@ -3995,16 +3977,16 @@
         <v>59</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L46" s="4" t="n">
         <v>0.305988215559662</v>
       </c>
       <c r="R46" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S46" s="4" t="n">
         <v>2013</v>
@@ -4015,10 +3997,10 @@
         <v>59</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L47" s="4" t="n">
         <v>3.43079190132787</v>
@@ -4035,10 +4017,10 @@
         <v>59</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L48" s="4" t="n">
         <v>3.34609968866095</v>
@@ -4055,10 +4037,10 @@
         <v>59</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L49" s="4" t="n">
         <v>3.92845513835257</v>
@@ -4075,10 +4057,10 @@
         <v>64</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L50" s="4" t="n">
         <v>24.4178275844343</v>
@@ -4095,10 +4077,10 @@
         <v>64</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L51" s="4" t="n">
         <v>22.1264702457203</v>
@@ -4115,10 +4097,10 @@
         <v>64</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L52" s="4" t="n">
         <v>21.7361460669016</v>
@@ -4135,10 +4117,10 @@
         <v>64</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L53" s="4" t="n">
         <v>3.56694094280734</v>
@@ -4155,10 +4137,10 @@
         <v>64</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L54" s="4" t="n">
         <v>3.5650623885918</v>
@@ -4175,10 +4157,10 @@
         <v>64</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L55" s="4" t="n">
         <v>3.68367295681731</v>
@@ -4195,16 +4177,16 @@
         <v>64</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L56" s="4" t="n">
         <v>1.35192141831578</v>
       </c>
       <c r="R56" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S56" s="4" t="n">
         <v>2011</v>
@@ -4215,16 +4197,16 @@
         <v>64</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L57" s="4" t="n">
         <v>1.35754114103847</v>
       </c>
       <c r="R57" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S57" s="4" t="n">
         <v>2012</v>
@@ -4235,16 +4217,16 @@
         <v>64</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L58" s="4" t="n">
         <v>1.38019522094625</v>
       </c>
       <c r="R58" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S58" s="4" t="n">
         <v>2013</v>
@@ -4255,10 +4237,10 @@
         <v>64</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L59" s="4" t="n">
         <v>52.3453630732544</v>
@@ -4275,10 +4257,10 @@
         <v>64</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L60" s="4" t="n">
         <v>51.2674451723156</v>
@@ -4295,10 +4277,10 @@
         <v>64</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L61" s="4" t="n">
         <v>60.9116442759974</v>
@@ -4315,10 +4297,10 @@
         <v>66</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L62" s="4" t="n">
         <v>1.15663393821004</v>
@@ -4335,10 +4317,10 @@
         <v>66</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L63" s="4" t="n">
         <v>1.0480959590078</v>
@@ -4355,10 +4337,10 @@
         <v>66</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L64" s="4" t="n">
         <v>1.0296069189585</v>
@@ -4375,10 +4357,10 @@
         <v>66</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L65" s="4" t="n">
         <v>2.43200518827774</v>
@@ -4395,10 +4377,10 @@
         <v>66</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L66" s="4" t="n">
         <v>2.43072435585805</v>
@@ -4415,10 +4397,10 @@
         <v>66</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L67" s="4" t="n">
         <v>2.51159519782998</v>
@@ -4435,16 +4417,16 @@
         <v>66</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L68" s="4" t="n">
         <v>0.625889545516565</v>
       </c>
       <c r="R68" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S68" s="4" t="n">
         <v>2011</v>
@@ -4455,16 +4437,16 @@
         <v>66</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L69" s="4" t="n">
         <v>0.628491268999291</v>
       </c>
       <c r="R69" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S69" s="4" t="n">
         <v>2012</v>
@@ -4475,16 +4457,16 @@
         <v>66</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L70" s="4" t="n">
         <v>0.638979268956598</v>
       </c>
       <c r="R70" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S70" s="4" t="n">
         <v>2013</v>
@@ -4495,10 +4477,10 @@
         <v>66</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L71" s="4" t="n">
         <v>7.27018931572978</v>
@@ -4515,10 +4497,10 @@
         <v>66</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L72" s="4" t="n">
         <v>7.12047849615494</v>
@@ -4535,10 +4517,10 @@
         <v>66</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L73" s="4" t="n">
         <v>8.45995059388853</v>
@@ -4555,10 +4537,10 @@
         <v>68</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L74" s="4" t="n">
         <v>1.28514882023338</v>
@@ -4575,10 +4557,10 @@
         <v>68</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L75" s="4" t="n">
         <v>1.16455106556423</v>
@@ -4595,10 +4577,10 @@
         <v>68</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L76" s="4" t="n">
         <v>1.14400768773166</v>
@@ -4615,10 +4597,10 @@
         <v>68</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L77" s="4" t="n">
         <v>1.62133679218516</v>
@@ -4635,10 +4617,10 @@
         <v>68</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L78" s="4" t="n">
         <v>1.62048290390536</v>
@@ -4655,10 +4637,10 @@
         <v>68</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L79" s="4" t="n">
         <v>1.67439679855332</v>
@@ -4675,16 +4657,16 @@
         <v>68</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L80" s="4" t="n">
         <v>0.876245363723192</v>
       </c>
       <c r="R80" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S80" s="4" t="n">
         <v>2011</v>
@@ -4695,16 +4677,16 @@
         <v>68</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L81" s="4" t="n">
         <v>0.879887776599008</v>
       </c>
       <c r="R81" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S81" s="4" t="n">
         <v>2012</v>
@@ -4715,16 +4697,16 @@
         <v>68</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L82" s="4" t="n">
         <v>0.894570976539237</v>
       </c>
       <c r="R82" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S82" s="4" t="n">
         <v>2013</v>
@@ -4735,10 +4717,10 @@
         <v>68</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L83" s="4" t="n">
         <v>8.72422717887574</v>
@@ -4755,10 +4737,10 @@
         <v>68</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L84" s="4" t="n">
         <v>8.54457419538593</v>
@@ -4775,10 +4757,10 @@
         <v>68</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L85" s="4" t="n">
         <v>10.1519407126662</v>
@@ -4795,10 +4777,10 @@
         <v>70</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L86" s="4" t="n">
         <v>11.7274304598456</v>
@@ -4815,10 +4797,10 @@
         <v>70</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L87" s="4" t="n">
         <v>7.47666590379534</v>
@@ -4835,10 +4817,10 @@
         <v>70</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L88" s="4" t="n">
         <v>1.2054039882177</v>
@@ -4855,10 +4837,10 @@
         <v>70</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L89" s="4" t="n">
         <v>24.1961621014873</v>
@@ -4875,10 +4857,10 @@
         <v>70</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L90" s="4" t="n">
         <v>10.6269339576279</v>
@@ -4895,10 +4877,10 @@
         <v>70</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L91" s="4" t="n">
         <v>7.47272826578086</v>
@@ -4915,16 +4897,16 @@
         <v>70</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L92" s="4" t="n">
         <v>1.21041466124265</v>
       </c>
       <c r="R92" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S92" s="4" t="n">
         <v>2011</v>
@@ -4935,16 +4917,16 @@
         <v>70</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L93" s="4" t="n">
         <v>23.6979044768967</v>
       </c>
       <c r="R93" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S93" s="4" t="n">
         <v>2012</v>
@@ -4955,16 +4937,16 @@
         <v>70</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L94" s="4" t="n">
         <v>10.439468481919</v>
       </c>
       <c r="R94" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S94" s="4" t="n">
         <v>2013</v>
@@ -4975,10 +4957,10 @@
         <v>70</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L95" s="4" t="n">
         <v>7.7213479108775</v>
@@ -4995,10 +4977,10 @@
         <v>70</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L96" s="4" t="n">
         <v>1.23061355586794</v>
@@ -5015,10 +4997,10 @@
         <v>70</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L97" s="4" t="n">
         <v>28.1558467119165</v>
@@ -5048,8 +5030,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I17" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R31" activeCellId="0" sqref="R31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5085,7 +5067,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>79</v>
@@ -5097,7 +5079,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>31</v>
@@ -5109,7 +5091,7 @@
         <v>90</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>3</v>
@@ -5118,31 +5100,31 @@
         <v>30</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -5150,12 +5132,12 @@
       <c r="B2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>14.639493</v>
@@ -5164,19 +5146,19 @@
         <v>47</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>7.7147</v>
@@ -5185,7 +5167,7 @@
         <v>47</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5193,10 +5175,10 @@
         <v>59</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>1.4</v>
@@ -5205,7 +5187,7 @@
         <v>47</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5213,10 +5195,10 @@
         <v>72</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>52.14</v>
@@ -5225,7 +5207,7 @@
         <v>47</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5233,10 +5215,10 @@
         <v>75</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>1077.676</v>
@@ -5245,27 +5227,27 @@
         <v>47</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="14" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L7" s="15" t="n">
+        <v>111</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L7" s="13" t="n">
         <v>4.7689</v>
       </c>
-      <c r="R7" s="15" t="s">
+      <c r="R7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="S7" s="15" t="s">
-        <v>139</v>
+      <c r="S7" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="AMJ7" s="0"/>
     </row>
@@ -5274,19 +5256,19 @@
         <v>57</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>0.423619</v>
       </c>
-      <c r="R8" s="17" t="s">
+      <c r="R8" s="15" t="s">
         <v>47</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5294,19 +5276,19 @@
         <v>57</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L9" s="0" t="n">
         <v>0.198178</v>
       </c>
-      <c r="R9" s="17" t="s">
+      <c r="R9" s="15" t="s">
         <v>47</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5314,19 +5296,19 @@
         <v>59</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L10" s="0" t="n">
         <v>0.7</v>
       </c>
-      <c r="R10" s="17" t="s">
+      <c r="R10" s="15" t="s">
         <v>47</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5334,19 +5316,19 @@
         <v>72</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>201.02</v>
       </c>
-      <c r="R11" s="17" t="s">
+      <c r="R11" s="15" t="s">
         <v>47</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5354,39 +5336,39 @@
         <v>75</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>1245.42</v>
       </c>
-      <c r="R12" s="17" t="s">
+      <c r="R12" s="15" t="s">
         <v>47</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L13" s="15" t="n">
+        <v>113</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L13" s="13" t="n">
         <v>2.690051</v>
       </c>
-      <c r="R13" s="15" t="s">
+      <c r="R13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="S13" s="15" t="s">
-        <v>139</v>
+      <c r="S13" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="AMJ13" s="0"/>
     </row>
@@ -5395,10 +5377,10 @@
         <v>57</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L14" s="0" t="n">
         <v>0.483017507961291</v>
@@ -5407,7 +5389,7 @@
         <v>47</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5415,10 +5397,10 @@
         <v>57</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L15" s="0" t="n">
         <v>0.318721995608352</v>
@@ -5427,7 +5409,7 @@
         <v>47</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5435,10 +5417,10 @@
         <v>59</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>0.7</v>
@@ -5447,7 +5429,7 @@
         <v>47</v>
       </c>
       <c r="S16" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5455,10 +5437,10 @@
         <v>72</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>139.440647380989</v>
@@ -5467,7 +5449,7 @@
         <v>47</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5475,10 +5457,10 @@
         <v>75</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L18" s="0" t="n">
         <v>2886.98274968357</v>
@@ -5487,27 +5469,27 @@
         <v>47</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L19" s="15" t="n">
+        <v>115</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L19" s="13" t="n">
         <v>4.94047619047619</v>
       </c>
-      <c r="R19" s="15" t="s">
+      <c r="R19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="S19" s="15" t="s">
-        <v>139</v>
+      <c r="S19" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="AMJ19" s="0"/>
     </row>
@@ -5516,10 +5498,10 @@
         <v>57</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L20" s="0" t="n">
         <v>31.1</v>
@@ -5528,7 +5510,7 @@
         <v>46</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5536,10 +5518,10 @@
         <v>57</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L21" s="0" t="n">
         <v>21.2</v>
@@ -5548,7 +5530,7 @@
         <v>46</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5556,10 +5538,10 @@
         <v>59</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L22" s="0" t="n">
         <v>0.7</v>
@@ -5568,7 +5550,7 @@
         <v>46</v>
       </c>
       <c r="S22" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5576,10 +5558,10 @@
         <v>72</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L23" s="0" t="n">
         <v>143.0069</v>
@@ -5588,7 +5570,7 @@
         <v>46</v>
       </c>
       <c r="S23" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5596,10 +5578,10 @@
         <v>75</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L24" s="0" t="n">
         <v>562</v>
@@ -5608,27 +5590,27 @@
         <v>46</v>
       </c>
       <c r="S24" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L25" s="15" t="n">
+        <v>117</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L25" s="13" t="n">
         <v>15</v>
       </c>
-      <c r="R25" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="S25" s="15" t="s">
-        <v>139</v>
+      <c r="R25" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="S25" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="AMJ25" s="0"/>
     </row>
@@ -5637,10 +5619,10 @@
         <v>57</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L26" s="0" t="n">
         <v>11.000603</v>
@@ -5649,7 +5631,7 @@
         <v>46</v>
       </c>
       <c r="S26" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5657,10 +5639,10 @@
         <v>57</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L27" s="0" t="n">
         <v>1.1</v>
@@ -5669,7 +5651,7 @@
         <v>46</v>
       </c>
       <c r="S27" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5677,10 +5659,10 @@
         <v>59</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L28" s="0" t="n">
         <v>0.7</v>
@@ -5689,7 +5671,7 @@
         <v>46</v>
       </c>
       <c r="S28" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5697,10 +5679,10 @@
         <v>72</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L29" s="0" t="n">
         <v>218.0069</v>
@@ -5709,7 +5691,7 @@
         <v>46</v>
       </c>
       <c r="S29" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5717,10 +5699,10 @@
         <v>75</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L30" s="0" t="n">
         <v>5054</v>
@@ -5729,27 +5711,27 @@
         <v>46</v>
       </c>
       <c r="S30" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L31" s="15" t="n">
+        <v>119</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L31" s="13" t="n">
         <v>11.5</v>
       </c>
-      <c r="R31" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="S31" s="15" t="s">
-        <v>139</v>
+      <c r="R31" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="S31" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="AMJ31" s="0"/>
     </row>
@@ -5758,10 +5740,10 @@
         <v>57</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L32" s="0" t="n">
         <v>4.388</v>
@@ -5770,7 +5752,7 @@
         <v>46</v>
       </c>
       <c r="S32" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5778,10 +5760,10 @@
         <v>57</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L33" s="0" t="n">
         <v>4.34</v>
@@ -5790,7 +5772,7 @@
         <v>46</v>
       </c>
       <c r="S33" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5798,10 +5780,10 @@
         <v>59</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L34" s="0" t="n">
         <v>0.7</v>
@@ -5810,7 +5792,7 @@
         <v>46</v>
       </c>
       <c r="S34" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5818,10 +5800,10 @@
         <v>72</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L35" s="0" t="n">
         <v>421.0069</v>
@@ -5830,7 +5812,7 @@
         <v>46</v>
       </c>
       <c r="S35" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5838,10 +5820,10 @@
         <v>75</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L36" s="0" t="n">
         <v>14662</v>
@@ -5850,27 +5832,27 @@
         <v>46</v>
       </c>
       <c r="S36" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="14" t="s">
         <v>42</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L37" s="15" t="n">
+        <v>121</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L37" s="13" t="n">
         <v>3.4</v>
       </c>
-      <c r="R37" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="S37" s="15" t="s">
-        <v>139</v>
+      <c r="R37" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="S37" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="AMJ37" s="0"/>
     </row>
@@ -5879,10 +5861,10 @@
         <v>57</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L38" s="0" t="n">
         <v>8.69</v>
@@ -5891,7 +5873,7 @@
         <v>46</v>
       </c>
       <c r="S38" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5899,10 +5881,10 @@
         <v>57</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L39" s="0" t="n">
         <v>2.79</v>
@@ -5911,7 +5893,7 @@
         <v>46</v>
       </c>
       <c r="S39" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5919,10 +5901,10 @@
         <v>59</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L40" s="0" t="n">
         <v>0.7</v>
@@ -5931,7 +5913,7 @@
         <v>46</v>
       </c>
       <c r="S40" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5939,10 +5921,10 @@
         <v>72</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L41" s="0" t="n">
         <v>407.0069</v>
@@ -5951,7 +5933,7 @@
         <v>46</v>
       </c>
       <c r="S41" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5959,10 +5941,10 @@
         <v>75</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L42" s="0" t="n">
         <v>14562</v>
@@ -5971,7 +5953,7 @@
         <v>46</v>
       </c>
       <c r="S42" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5979,10 +5961,10 @@
         <v>43</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L43" s="0" t="n">
         <v>3.26</v>
@@ -5991,7 +5973,7 @@
         <v>46</v>
       </c>
       <c r="S43" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -6035,37 +6017,37 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>152</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>6</v>
@@ -6073,115 +6055,115 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>43</v>
@@ -6189,7 +6171,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -6199,7 +6181,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>47</v>
@@ -6211,29 +6193,29 @@
         <v>47</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>47</v>
@@ -6245,12 +6227,12 @@
         <v>47</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>46</v>
@@ -6262,12 +6244,12 @@
         <v>46</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>46</v>
@@ -6279,12 +6261,12 @@
         <v>46</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>46</v>
@@ -6296,12 +6278,12 @@
         <v>46</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>46</v>
@@ -6315,7 +6297,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -6337,10 +6319,10 @@
         <v>46</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6357,10 +6339,10 @@
         <v>47</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6377,7 +6359,7 @@
         <v>46</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6394,7 +6376,7 @@
         <v>47</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6411,9 +6393,9 @@
         <v>46</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="I20" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="I20" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6431,7 +6413,7 @@
         <v>47</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>12</v>
@@ -6472,36 +6454,36 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>47</v>
@@ -6518,10 +6500,10 @@
         <v>106</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>47</v>
@@ -6535,19 +6517,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="G4" s="4" t="n">
         <v>0.4</v>
@@ -6555,13 +6537,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>47</v>
@@ -6575,13 +6557,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>47</v>
@@ -6598,10 +6580,10 @@
         <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>47</v>
@@ -6615,13 +6597,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>46</v>
@@ -6638,10 +6620,10 @@
         <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>46</v>
@@ -6655,13 +6637,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>46</v>
@@ -6678,10 +6660,10 @@
         <v>41</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>46</v>
@@ -6695,13 +6677,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>46</v>
@@ -6718,10 +6700,10 @@
         <v>42</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>46</v>
@@ -6735,13 +6717,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>46</v>
@@ -6758,10 +6740,10 @@
         <v>43</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>46</v>
@@ -6782,19 +6764,19 @@
         <v>42</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6805,7 +6787,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>46</v>
@@ -6814,10 +6796,10 @@
         <v>46</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6828,7 +6810,7 @@
         <v>42</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>46</v>
@@ -6840,7 +6822,7 @@
         <v>42</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6851,7 +6833,7 @@
         <v>43</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>46</v>
@@ -6863,7 +6845,7 @@
         <v>43</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6874,7 +6856,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>46</v>
@@ -6883,10 +6865,10 @@
         <v>46</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6897,7 +6879,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>46</v>
@@ -6906,10 +6888,10 @@
         <v>46</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6920,7 +6902,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>46</v>
@@ -6932,7 +6914,7 @@
         <v>40</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6943,7 +6925,7 @@
         <v>41</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>46</v>
@@ -6955,7 +6937,7 @@
         <v>41</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6966,7 +6948,7 @@
         <v>106</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>47</v>
@@ -6975,10 +6957,10 @@
         <v>47</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6986,10 +6968,10 @@
         <v>104</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>47</v>
@@ -6998,10 +6980,10 @@
         <v>47</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7012,7 +6994,7 @@
         <v>39</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>47</v>
@@ -7021,10 +7003,10 @@
         <v>47</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7035,7 +7017,7 @@
         <v>106</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>47</v>
@@ -7047,7 +7029,7 @@
         <v>106</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7055,10 +7037,10 @@
         <v>104</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>47</v>
@@ -7067,10 +7049,10 @@
         <v>47</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7081,7 +7063,7 @@
         <v>39</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>47</v>
@@ -7093,7 +7075,7 @@
         <v>39</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7104,7 +7086,7 @@
         <v>102</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>46</v>
@@ -7124,7 +7106,7 @@
         <v>103</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>46</v>
@@ -7145,7 +7127,7 @@
         <v>104</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Support for expansion of macros, implemented in BareProcessors command
* BasicCommand: major feature, settling the support for expansion of macros, so Commands only need to implement "_process_row"
* DatasetQryCommand: now creates a new Dataset object using the dimensions and measures of the output, and custom code lists (only those appearing in the resulting Dataframe)
  * Cython (Pyximport) to use "language_level=3 for Python 3
* ProcessorScalingsCommand: Fixed "from" statement
* ProcessorsCommand: use "BasicCommand" as base class, only _process_row and proper __init__ialization
* "parser_field_parsers.py": changes to remove use of curly braces in all syntactic rules, which are now reserved to macro expansion
* "parse_command_in_worksheet" function enhanced to delegate syntactic validation when macro expansion is used
* requirements.txt: update of Flask, Werkzeug, requests, SQLAlchemy
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/Biofuel_NIS.xlsx
+++ b/backend_tests/z_input_files/v2/Biofuel_NIS.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="182">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -469,9 +469,6 @@
   </si>
   <si>
     <t xml:space="preserve">RelationType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChangeOfTypeScale</t>
   </si>
   <si>
     <t xml:space="preserve">Weight</t>
@@ -751,12 +748,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -768,7 +765,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -913,8 +910,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -926,7 +923,7 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1244,8 +1241,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1257,7 +1254,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1749,8 +1746,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1762,7 +1759,7 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2402,8 +2399,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2415,7 +2412,7 @@
   </sheetPr>
   <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -3000,8 +2997,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3013,7 +3010,7 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -5017,8 +5014,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5030,7 +5027,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -6021,8 +6018,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6034,8 +6031,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6045,13 +6042,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="18.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="15.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="4" width="15.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="15.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="10" style="4" width="15.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6080,11 +6076,9 @@
         <v>149</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
@@ -6102,7 +6096,7 @@
         <v>37</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6119,7 +6113,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6136,7 +6130,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6153,7 +6147,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6170,7 +6164,7 @@
         <v>41</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6187,7 +6181,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6204,13 +6198,12 @@
         <v>43</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
@@ -6226,7 +6219,7 @@
         <v>47</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6243,7 +6236,7 @@
         <v>47</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6260,7 +6253,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6277,7 +6270,7 @@
         <v>46</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6294,7 +6287,7 @@
         <v>46</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6311,7 +6304,7 @@
         <v>46</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6328,13 +6321,12 @@
         <v>46</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
@@ -6350,10 +6342,10 @@
         <v>46</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6370,10 +6362,10 @@
         <v>47</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6390,7 +6382,7 @@
         <v>46</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6407,7 +6399,7 @@
         <v>47</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6424,9 +6416,9 @@
         <v>46</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G20" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6444,9 +6436,9 @@
         <v>47</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G21" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6455,8 +6447,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6468,7 +6460,7 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6485,25 +6477,25 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6514,7 +6506,7 @@
         <v>111</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>47</v>
@@ -6534,7 +6526,7 @@
         <v>113</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>47</v>
@@ -6554,7 +6546,7 @@
         <v>115</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>47</v>
@@ -6574,7 +6566,7 @@
         <v>117</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>46</v>
@@ -6594,7 +6586,7 @@
         <v>119</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>46</v>
@@ -6614,7 +6606,7 @@
         <v>121</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>46</v>
@@ -6634,7 +6626,7 @@
         <v>123</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>46</v>
@@ -6655,19 +6647,19 @@
         <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6678,7 +6670,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>46</v>
@@ -6687,10 +6679,10 @@
         <v>46</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6701,7 +6693,7 @@
         <v>42</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>46</v>
@@ -6713,7 +6705,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6724,7 +6716,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>46</v>
@@ -6736,7 +6728,7 @@
         <v>43</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6747,7 +6739,7 @@
         <v>40</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>46</v>
@@ -6756,10 +6748,10 @@
         <v>46</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6770,7 +6762,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>46</v>
@@ -6779,10 +6771,10 @@
         <v>46</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6793,7 +6785,7 @@
         <v>40</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>46</v>
@@ -6805,7 +6797,7 @@
         <v>40</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6816,7 +6808,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>46</v>
@@ -6828,7 +6820,7 @@
         <v>41</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6839,7 +6831,7 @@
         <v>106</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>47</v>
@@ -6848,10 +6840,10 @@
         <v>47</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6862,7 +6854,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>47</v>
@@ -6871,10 +6863,10 @@
         <v>47</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6885,7 +6877,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>47</v>
@@ -6894,10 +6886,10 @@
         <v>47</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6908,7 +6900,7 @@
         <v>106</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>47</v>
@@ -6920,7 +6912,7 @@
         <v>106</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6931,7 +6923,7 @@
         <v>38</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>47</v>
@@ -6943,7 +6935,7 @@
         <v>38</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6954,7 +6946,7 @@
         <v>39</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>47</v>
@@ -6966,7 +6958,7 @@
         <v>39</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6977,7 +6969,7 @@
         <v>102</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>46</v>
@@ -6997,7 +6989,7 @@
         <v>103</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>46</v>
@@ -7018,7 +7010,7 @@
         <v>104</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>47</v>
@@ -7035,8 +7027,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>